<commit_message>
Bajada de sap parseada
</commit_message>
<xml_diff>
--- a/bajada_sap2.xlsx
+++ b/bajada_sap2.xlsx
@@ -917,7 +917,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:V578"/>
+  <dimension ref="B2:V999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3954,6 +3954,7 @@
         <v>-13.36</v>
       </c>
     </row>
+    <row r="56"/>
     <row r="57">
       <c r="B57" t="n">
         <v>10002768</v>
@@ -12539,6 +12540,7 @@
         <v>-19.96</v>
       </c>
     </row>
+    <row r="202"/>
     <row r="203">
       <c r="B203" t="n">
         <v>10002769</v>
@@ -14793,6 +14795,7 @@
         <v>16.98</v>
       </c>
     </row>
+    <row r="242"/>
     <row r="243">
       <c r="B243" t="n">
         <v>10002770</v>
@@ -32276,6 +32279,7 @@
         <v>8.4</v>
       </c>
     </row>
+    <row r="535"/>
     <row r="536">
       <c r="B536" t="n">
         <v>10002771</v>
@@ -33993,6 +33997,7 @@
         <v>18.38</v>
       </c>
     </row>
+    <row r="566"/>
     <row r="567">
       <c r="B567" t="n">
         <v>10002774</v>
@@ -34658,6 +34663,427 @@
         <v>-11.16</v>
       </c>
     </row>
+    <row r="579"/>
+    <row r="580"/>
+    <row r="581"/>
+    <row r="582"/>
+    <row r="583"/>
+    <row r="584"/>
+    <row r="585"/>
+    <row r="586"/>
+    <row r="587"/>
+    <row r="588"/>
+    <row r="589"/>
+    <row r="590"/>
+    <row r="591"/>
+    <row r="592"/>
+    <row r="593"/>
+    <row r="594"/>
+    <row r="595"/>
+    <row r="596"/>
+    <row r="597"/>
+    <row r="598"/>
+    <row r="599"/>
+    <row r="600"/>
+    <row r="601"/>
+    <row r="602"/>
+    <row r="603"/>
+    <row r="604"/>
+    <row r="605"/>
+    <row r="606"/>
+    <row r="607"/>
+    <row r="608"/>
+    <row r="609"/>
+    <row r="610"/>
+    <row r="611"/>
+    <row r="612"/>
+    <row r="613"/>
+    <row r="614"/>
+    <row r="615"/>
+    <row r="616"/>
+    <row r="617"/>
+    <row r="618"/>
+    <row r="619"/>
+    <row r="620"/>
+    <row r="621"/>
+    <row r="622"/>
+    <row r="623"/>
+    <row r="624"/>
+    <row r="625"/>
+    <row r="626"/>
+    <row r="627"/>
+    <row r="628"/>
+    <row r="629"/>
+    <row r="630"/>
+    <row r="631"/>
+    <row r="632"/>
+    <row r="633"/>
+    <row r="634"/>
+    <row r="635"/>
+    <row r="636"/>
+    <row r="637"/>
+    <row r="638"/>
+    <row r="639"/>
+    <row r="640"/>
+    <row r="641"/>
+    <row r="642"/>
+    <row r="643"/>
+    <row r="644"/>
+    <row r="645"/>
+    <row r="646"/>
+    <row r="647"/>
+    <row r="648"/>
+    <row r="649"/>
+    <row r="650"/>
+    <row r="651"/>
+    <row r="652"/>
+    <row r="653"/>
+    <row r="654"/>
+    <row r="655"/>
+    <row r="656"/>
+    <row r="657"/>
+    <row r="658"/>
+    <row r="659"/>
+    <row r="660"/>
+    <row r="661"/>
+    <row r="662"/>
+    <row r="663"/>
+    <row r="664"/>
+    <row r="665"/>
+    <row r="666"/>
+    <row r="667"/>
+    <row r="668"/>
+    <row r="669"/>
+    <row r="670"/>
+    <row r="671"/>
+    <row r="672"/>
+    <row r="673"/>
+    <row r="674"/>
+    <row r="675"/>
+    <row r="676"/>
+    <row r="677"/>
+    <row r="678"/>
+    <row r="679"/>
+    <row r="680"/>
+    <row r="681"/>
+    <row r="682"/>
+    <row r="683"/>
+    <row r="684"/>
+    <row r="685"/>
+    <row r="686"/>
+    <row r="687"/>
+    <row r="688"/>
+    <row r="689"/>
+    <row r="690"/>
+    <row r="691"/>
+    <row r="692"/>
+    <row r="693"/>
+    <row r="694"/>
+    <row r="695"/>
+    <row r="696"/>
+    <row r="697"/>
+    <row r="698"/>
+    <row r="699"/>
+    <row r="700"/>
+    <row r="701"/>
+    <row r="702"/>
+    <row r="703"/>
+    <row r="704"/>
+    <row r="705"/>
+    <row r="706"/>
+    <row r="707"/>
+    <row r="708"/>
+    <row r="709"/>
+    <row r="710"/>
+    <row r="711"/>
+    <row r="712"/>
+    <row r="713"/>
+    <row r="714"/>
+    <row r="715"/>
+    <row r="716"/>
+    <row r="717"/>
+    <row r="718"/>
+    <row r="719"/>
+    <row r="720"/>
+    <row r="721"/>
+    <row r="722"/>
+    <row r="723"/>
+    <row r="724"/>
+    <row r="725"/>
+    <row r="726"/>
+    <row r="727"/>
+    <row r="728"/>
+    <row r="729"/>
+    <row r="730"/>
+    <row r="731"/>
+    <row r="732"/>
+    <row r="733"/>
+    <row r="734"/>
+    <row r="735"/>
+    <row r="736"/>
+    <row r="737"/>
+    <row r="738"/>
+    <row r="739"/>
+    <row r="740"/>
+    <row r="741"/>
+    <row r="742"/>
+    <row r="743"/>
+    <row r="744"/>
+    <row r="745"/>
+    <row r="746"/>
+    <row r="747"/>
+    <row r="748"/>
+    <row r="749"/>
+    <row r="750"/>
+    <row r="751"/>
+    <row r="752"/>
+    <row r="753"/>
+    <row r="754"/>
+    <row r="755"/>
+    <row r="756"/>
+    <row r="757"/>
+    <row r="758"/>
+    <row r="759"/>
+    <row r="760"/>
+    <row r="761"/>
+    <row r="762"/>
+    <row r="763"/>
+    <row r="764"/>
+    <row r="765"/>
+    <row r="766"/>
+    <row r="767"/>
+    <row r="768"/>
+    <row r="769"/>
+    <row r="770"/>
+    <row r="771"/>
+    <row r="772"/>
+    <row r="773"/>
+    <row r="774"/>
+    <row r="775"/>
+    <row r="776"/>
+    <row r="777"/>
+    <row r="778"/>
+    <row r="779"/>
+    <row r="780"/>
+    <row r="781"/>
+    <row r="782"/>
+    <row r="783"/>
+    <row r="784"/>
+    <row r="785"/>
+    <row r="786"/>
+    <row r="787"/>
+    <row r="788"/>
+    <row r="789"/>
+    <row r="790"/>
+    <row r="791"/>
+    <row r="792"/>
+    <row r="793"/>
+    <row r="794"/>
+    <row r="795"/>
+    <row r="796"/>
+    <row r="797"/>
+    <row r="798"/>
+    <row r="799"/>
+    <row r="800"/>
+    <row r="801"/>
+    <row r="802"/>
+    <row r="803"/>
+    <row r="804"/>
+    <row r="805"/>
+    <row r="806"/>
+    <row r="807"/>
+    <row r="808"/>
+    <row r="809"/>
+    <row r="810"/>
+    <row r="811"/>
+    <row r="812"/>
+    <row r="813"/>
+    <row r="814"/>
+    <row r="815"/>
+    <row r="816"/>
+    <row r="817"/>
+    <row r="818"/>
+    <row r="819"/>
+    <row r="820"/>
+    <row r="821"/>
+    <row r="822"/>
+    <row r="823"/>
+    <row r="824"/>
+    <row r="825"/>
+    <row r="826"/>
+    <row r="827"/>
+    <row r="828"/>
+    <row r="829"/>
+    <row r="830"/>
+    <row r="831"/>
+    <row r="832"/>
+    <row r="833"/>
+    <row r="834"/>
+    <row r="835"/>
+    <row r="836"/>
+    <row r="837"/>
+    <row r="838"/>
+    <row r="839"/>
+    <row r="840"/>
+    <row r="841"/>
+    <row r="842"/>
+    <row r="843"/>
+    <row r="844"/>
+    <row r="845"/>
+    <row r="846"/>
+    <row r="847"/>
+    <row r="848"/>
+    <row r="849"/>
+    <row r="850"/>
+    <row r="851"/>
+    <row r="852"/>
+    <row r="853"/>
+    <row r="854"/>
+    <row r="855"/>
+    <row r="856"/>
+    <row r="857"/>
+    <row r="858"/>
+    <row r="859"/>
+    <row r="860"/>
+    <row r="861"/>
+    <row r="862"/>
+    <row r="863"/>
+    <row r="864"/>
+    <row r="865"/>
+    <row r="866"/>
+    <row r="867"/>
+    <row r="868"/>
+    <row r="869"/>
+    <row r="870"/>
+    <row r="871"/>
+    <row r="872"/>
+    <row r="873"/>
+    <row r="874"/>
+    <row r="875"/>
+    <row r="876"/>
+    <row r="877"/>
+    <row r="878"/>
+    <row r="879"/>
+    <row r="880"/>
+    <row r="881"/>
+    <row r="882"/>
+    <row r="883"/>
+    <row r="884"/>
+    <row r="885"/>
+    <row r="886"/>
+    <row r="887"/>
+    <row r="888"/>
+    <row r="889"/>
+    <row r="890"/>
+    <row r="891"/>
+    <row r="892"/>
+    <row r="893"/>
+    <row r="894"/>
+    <row r="895"/>
+    <row r="896"/>
+    <row r="897"/>
+    <row r="898"/>
+    <row r="899"/>
+    <row r="900"/>
+    <row r="901"/>
+    <row r="902"/>
+    <row r="903"/>
+    <row r="904"/>
+    <row r="905"/>
+    <row r="906"/>
+    <row r="907"/>
+    <row r="908"/>
+    <row r="909"/>
+    <row r="910"/>
+    <row r="911"/>
+    <row r="912"/>
+    <row r="913"/>
+    <row r="914"/>
+    <row r="915"/>
+    <row r="916"/>
+    <row r="917"/>
+    <row r="918"/>
+    <row r="919"/>
+    <row r="920"/>
+    <row r="921"/>
+    <row r="922"/>
+    <row r="923"/>
+    <row r="924"/>
+    <row r="925"/>
+    <row r="926"/>
+    <row r="927"/>
+    <row r="928"/>
+    <row r="929"/>
+    <row r="930"/>
+    <row r="931"/>
+    <row r="932"/>
+    <row r="933"/>
+    <row r="934"/>
+    <row r="935"/>
+    <row r="936"/>
+    <row r="937"/>
+    <row r="938"/>
+    <row r="939"/>
+    <row r="940"/>
+    <row r="941"/>
+    <row r="942"/>
+    <row r="943"/>
+    <row r="944"/>
+    <row r="945"/>
+    <row r="946"/>
+    <row r="947"/>
+    <row r="948"/>
+    <row r="949"/>
+    <row r="950"/>
+    <row r="951"/>
+    <row r="952"/>
+    <row r="953"/>
+    <row r="954"/>
+    <row r="955"/>
+    <row r="956"/>
+    <row r="957"/>
+    <row r="958"/>
+    <row r="959"/>
+    <row r="960"/>
+    <row r="961"/>
+    <row r="962"/>
+    <row r="963"/>
+    <row r="964"/>
+    <row r="965"/>
+    <row r="966"/>
+    <row r="967"/>
+    <row r="968"/>
+    <row r="969"/>
+    <row r="970"/>
+    <row r="971"/>
+    <row r="972"/>
+    <row r="973"/>
+    <row r="974"/>
+    <row r="975"/>
+    <row r="976"/>
+    <row r="977"/>
+    <row r="978"/>
+    <row r="979"/>
+    <row r="980"/>
+    <row r="981"/>
+    <row r="982"/>
+    <row r="983"/>
+    <row r="984"/>
+    <row r="985"/>
+    <row r="986"/>
+    <row r="987"/>
+    <row r="988"/>
+    <row r="989"/>
+    <row r="990"/>
+    <row r="991"/>
+    <row r="992"/>
+    <row r="993"/>
+    <row r="994"/>
+    <row r="995"/>
+    <row r="996"/>
+    <row r="997"/>
+    <row r="998"/>
+    <row r="999"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34669,7 +35095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A6:A24"/>
+  <dimension ref="A1:F240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34677,99 +35103,4342 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>541</v>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>10002766</v>
+      </c>
+      <c r="B1" t="n">
+        <v>67364</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>20.03.2023</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F1" t="n">
+        <v>9.960000000000001</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>10002766</v>
+      </c>
+      <c r="B2" t="n">
+        <v>67409</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F2" t="n">
+        <v>8.539999999999999</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10002766</v>
+      </c>
+      <c r="B3" t="n">
+        <v>67410</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10002766</v>
+      </c>
+      <c r="B4" t="n">
+        <v>67366</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>20.03.2023</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7.06</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>10002766</v>
+      </c>
+      <c r="B5" t="n">
+        <v>67420</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F5" t="n">
+        <v>13.54</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>541</v>
+        <v>10002767</v>
+      </c>
+      <c r="B8" t="n">
+        <v>67387</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>31.03.2023</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12.28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>309</v>
+        <v>10002767</v>
+      </c>
+      <c r="B9" t="n">
+        <v>67391</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>03.04.2023</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>101</v>
+        <v>10002767</v>
+      </c>
+      <c r="B10" t="n">
+        <v>67404</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F10" t="n">
+        <v>11.86</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>541</v>
+        <v>10002767</v>
+      </c>
+      <c r="B11" t="n">
+        <v>67397</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F11" t="n">
+        <v>13.36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>541</v>
+        <v>10002767</v>
+      </c>
+      <c r="B12" t="n">
+        <v>67400</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F12" t="n">
+        <v>12.22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>309</v>
+        <v>10002767</v>
+      </c>
+      <c r="B13" t="n">
+        <v>67405</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F13" t="n">
+        <v>11.88</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>101</v>
+        <v>10002767</v>
+      </c>
+      <c r="B14" t="n">
+        <v>67406</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7.78</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>309</v>
+        <v>10002767</v>
+      </c>
+      <c r="B15" t="n">
+        <v>67408</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F15" t="n">
+        <v>6.14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>101</v>
+        <v>10002768</v>
+      </c>
+      <c r="B18" t="n">
+        <v>192070</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>28.03.2023</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>10012717</v>
+      </c>
+      <c r="F18" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>541</v>
+        <v>10002768</v>
+      </c>
+      <c r="B19" t="n">
+        <v>192070</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>28.03.2023</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>10012717</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>541</v>
+        <v>10002768</v>
+      </c>
+      <c r="B20" t="n">
+        <v>192069</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>28.03.2023</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>10012717</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10.08</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>309</v>
+        <v>10002768</v>
+      </c>
+      <c r="B21" t="n">
+        <v>12880</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>30.03.2023</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>10004686</v>
+      </c>
+      <c r="F21" t="n">
+        <v>20.14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>101</v>
+        <v>10002768</v>
+      </c>
+      <c r="B22" t="n">
+        <v>15454</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>30.03.2023</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>10008828</v>
+      </c>
+      <c r="F22" t="n">
+        <v>24.52</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>541</v>
+        <v>10002768</v>
+      </c>
+      <c r="B23" t="n">
+        <v>192087</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>01.04.2023</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>10010134</v>
+      </c>
+      <c r="F23" t="n">
+        <v>8.92</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>541</v>
+        <v>10002768</v>
+      </c>
+      <c r="B24" t="n">
+        <v>192088</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>01.04.2023</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F24" t="n">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B25" t="n">
+        <v>3084</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>03.04.2023</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>10012805</v>
+      </c>
+      <c r="F25" t="n">
+        <v>17.86</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B26" t="n">
+        <v>12881</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>03.04.2023</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>10004686</v>
+      </c>
+      <c r="F26" t="n">
+        <v>20.1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B27" t="n">
+        <v>172</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>09.02.2023</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>10012032</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-6.84</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B28" t="n">
+        <v>172</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>10.02.2023</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>10012032</v>
+      </c>
+      <c r="F28" t="n">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B29" t="n">
+        <v>12886</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>10004686</v>
+      </c>
+      <c r="F29" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B30" t="n">
+        <v>15614</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>10008828</v>
+      </c>
+      <c r="F30" t="n">
+        <v>19.76</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B31" t="n">
+        <v>192115</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>10012717</v>
+      </c>
+      <c r="F31" t="n">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B32" t="n">
+        <v>192103</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F32" t="n">
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B33" t="n">
+        <v>192103</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-9.82</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B34" t="n">
+        <v>215</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>10012032</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B35" t="n">
+        <v>214</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>10012032</v>
+      </c>
+      <c r="F35" t="n">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B36" t="n">
+        <v>218</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>10012279</v>
+      </c>
+      <c r="F36" t="n">
+        <v>6.46</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B37" t="n">
+        <v>29476</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>10004753</v>
+      </c>
+      <c r="F37" t="n">
+        <v>16.12</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B38" t="n">
+        <v>192484</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>10010134</v>
+      </c>
+      <c r="F38" t="n">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B39" t="n">
+        <v>192468</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>16.04.2023</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>10004464</v>
+      </c>
+      <c r="F39" t="n">
+        <v>11.62</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B40" t="n">
+        <v>192478</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>17.04.2023</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>10012717</v>
+      </c>
+      <c r="F40" t="n">
+        <v>7.12</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B41" t="n">
+        <v>192476</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>17.04.2023</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>10007342</v>
+      </c>
+      <c r="F41" t="n">
+        <v>9.02</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B42" t="n">
+        <v>3088</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>10012805</v>
+      </c>
+      <c r="F42" t="n">
+        <v>20.56</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B43" t="n">
+        <v>190947</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>22.02.2023</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>10010134</v>
+      </c>
+      <c r="F43" t="n">
+        <v>8.56</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B44" t="n">
+        <v>141251</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>17.04.2023</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>10004753</v>
+      </c>
+      <c r="F44" t="n">
+        <v>15.78</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B45" t="n">
+        <v>224</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>13.04.2023</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>10012032</v>
+      </c>
+      <c r="F45" t="n">
+        <v>5.34</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B46" t="n">
+        <v>192469</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>16.04.2023</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F46" t="n">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B47" t="n">
+        <v>192455</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>12.04.2023</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>10012201</v>
+      </c>
+      <c r="F47" t="n">
+        <v>8.42</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B48" t="n">
+        <v>192119</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>10012183</v>
+      </c>
+      <c r="F48" t="n">
+        <v>10.16</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B49" t="n">
+        <v>191719</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>21.03.2023</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>10012745</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B50" t="n">
+        <v>191720</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>21.03.2023</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>10004759</v>
+      </c>
+      <c r="F50" t="n">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B51" t="n">
+        <v>191329</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>06.03.2023</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>10012799</v>
+      </c>
+      <c r="F51" t="n">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B52" t="n">
+        <v>192080</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>29.03.2023</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>10011172</v>
+      </c>
+      <c r="F52" t="n">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B53" t="n">
+        <v>192453</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>12.04.2023</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>10004822</v>
+      </c>
+      <c r="F53" t="n">
+        <v>6.44</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B54" t="n">
+        <v>192086</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>01.04.2023</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>10012713</v>
+      </c>
+      <c r="F54" t="n">
+        <v>7.08</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B55" t="n">
+        <v>192109</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>10010134</v>
+      </c>
+      <c r="F55" t="n">
+        <v>9.58</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B56" t="n">
+        <v>192459</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>13.04.2023</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>10010134</v>
+      </c>
+      <c r="F56" t="n">
+        <v>9.74</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B57" t="n">
+        <v>192103</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F57" t="n">
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B58" t="n">
+        <v>192449</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F58" t="n">
+        <v>8.539999999999999</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B59" t="n">
+        <v>192127</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F59" t="n">
+        <v>10.34</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B60" t="n">
+        <v>191702</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>16.03.2023</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>10004777</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-6.76</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>FC7309</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>10004777</v>
+      </c>
+      <c r="F61" t="n">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B62" t="n">
+        <v>230</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>10012587</v>
+      </c>
+      <c r="F62" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B63" t="n">
+        <v>192489</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>19.04.2023</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F63" t="n">
+        <v>10.16</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B64" t="n">
+        <v>192508</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>24.04.2023</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F64" t="n">
+        <v>10.46</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B65" t="n">
+        <v>12896</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>10004686</v>
+      </c>
+      <c r="F65" t="n">
+        <v>19.96</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B66" t="n">
+        <v>192501</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>10005092</v>
+      </c>
+      <c r="F66" t="n">
+        <v>12.28</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B67" t="n">
+        <v>3</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>10010134</v>
+      </c>
+      <c r="F67" t="n">
+        <v>12.36</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B68" t="n">
+        <v>192519</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>25.04.2023</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>10012717</v>
+      </c>
+      <c r="F68" t="n">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B69" t="n">
+        <v>192498</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>10012183</v>
+      </c>
+      <c r="F69" t="n">
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B70" t="n">
+        <v>237</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>10012032</v>
+      </c>
+      <c r="F70" t="n">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B71" t="n">
+        <v>11534</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>10012279</v>
+      </c>
+      <c r="F71" t="n">
+        <v>4.76</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B72" t="n">
+        <v>192844</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F72" t="n">
+        <v>9.92</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B73" t="n">
+        <v>192845</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>10012201</v>
+      </c>
+      <c r="F73" t="n">
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B74" t="n">
+        <v>192844</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-9.92</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B75" t="n">
+        <v>192844</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F75" t="n">
+        <v>9.92</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B76" t="n">
+        <v>192845</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>10012201</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-9.82</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B77" t="n">
+        <v>192845</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>10012201</v>
+      </c>
+      <c r="F77" t="n">
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B78" t="n">
+        <v>192845</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>10012201</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-9.82</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B79" t="n">
+        <v>192845</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>10012201</v>
+      </c>
+      <c r="F79" t="n">
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B80" t="n">
+        <v>192845</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>10012201</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-9.82</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>10002768</v>
+      </c>
+      <c r="B81" t="n">
+        <v>192845</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>10012201</v>
+      </c>
+      <c r="F81" t="n">
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B84" t="n">
+        <v>8238</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>30.03.2023</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F84" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B85" t="n">
+        <v>8241</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>31.03.2023</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F85" t="n">
+        <v>19.78</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B86" t="n">
+        <v>8242</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>03.04.2023</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F86" t="n">
+        <v>19.46</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B87" t="n">
+        <v>8244</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>03.04.2023</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F87" t="n">
+        <v>18.82</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B88" t="n">
+        <v>8247</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>04.04.2023</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F88" t="n">
+        <v>19.28</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B89" t="n">
+        <v>8246</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>04.04.2023</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F89" t="n">
+        <v>19.18</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B90" t="n">
+        <v>8308</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F90" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B91" t="n">
+        <v>8249</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F91" t="n">
+        <v>17.82</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B92" t="n">
+        <v>8248</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F92" t="n">
+        <v>19.18</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B93" t="n">
+        <v>8302</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F93" t="n">
+        <v>18.36</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B94" t="n">
+        <v>8303</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F94" t="n">
+        <v>18.46</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B95" t="n">
+        <v>8250</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F95" t="n">
+        <v>18.26</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B96" t="n">
+        <v>8301</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F96" t="n">
+        <v>18.76</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B97" t="n">
+        <v>8304</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>07.04.2023</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F97" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B98" t="n">
+        <v>8305</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>07.04.2023</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F98" t="n">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B99" t="n">
+        <v>8306</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F99" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B100" t="n">
+        <v>8310</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F100" t="n">
+        <v>17.88</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B101" t="n">
+        <v>8309</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F101" t="n">
+        <v>17.46</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B102" t="n">
+        <v>8229</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>22.03.2023</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F102" t="n">
+        <v>19.14</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B103" t="n">
+        <v>8225</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>22.03.2023</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F103" t="n">
+        <v>18.04</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B104" t="n">
+        <v>8230</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>23.03.2023</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F104" t="n">
+        <v>19.28</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B105" t="n">
+        <v>8312</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>12.04.2023</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F105" t="n">
+        <v>18.06</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B106" t="n">
+        <v>8311</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>12.04.2023</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F106" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B107" t="n">
+        <v>8316</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>13.04.2023</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F107" t="n">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B108" t="n">
+        <v>8314</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>13.04.2023</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F108" t="n">
+        <v>17.54</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B109" t="n">
+        <v>8313</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>12.04.2023</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F109" t="n">
+        <v>17.72</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B110" t="n">
+        <v>8324</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F110" t="n">
+        <v>18.46</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B111" t="n">
+        <v>8325</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F111" t="n">
+        <v>18.52</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B112" t="n">
+        <v>8331</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>24.04.2023</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F112" t="n">
+        <v>18.28</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B113" t="n">
+        <v>8328</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>24.04.2023</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F113" t="n">
+        <v>18.62</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B114" t="n">
+        <v>8334</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F114" t="n">
+        <v>17.68</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B115" t="n">
+        <v>8335</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F115" t="n">
+        <v>17.86</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B116" t="n">
+        <v>8337</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F116" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B117" t="n">
+        <v>8338</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F117" t="n">
+        <v>18.16</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B118" t="n">
+        <v>8340</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>28.04.2023</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F118" t="n">
+        <v>17.28</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>10002769</v>
+      </c>
+      <c r="B119" t="n">
+        <v>8342</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>28.04.2023</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F119" t="n">
+        <v>16.98</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B122" t="n">
+        <v>192070</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>28.03.2023</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>10012717</v>
+      </c>
+      <c r="F122" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B123" t="n">
+        <v>192079</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>29.03.2023</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>10005092</v>
+      </c>
+      <c r="F123" t="n">
+        <v>9.539999999999999</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B124" t="n">
+        <v>192077</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>29.03.2023</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F124" t="n">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B125" t="n">
+        <v>211</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>30.03.2023</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>10012587</v>
+      </c>
+      <c r="F125" t="n">
+        <v>5.02</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B126" t="n">
+        <v>212</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>30.03.2023</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>10012587</v>
+      </c>
+      <c r="F126" t="n">
+        <v>7.74</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B127" t="n">
+        <v>29446</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>29.03.2023</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>10004753</v>
+      </c>
+      <c r="F127" t="n">
+        <v>24.68</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B128" t="n">
+        <v>15455</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>31.03.2023</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>10008828</v>
+      </c>
+      <c r="F128" t="n">
+        <v>28.56</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B129" t="n">
+        <v>4004</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>29.03.2023</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F129" t="n">
+        <v>9.34</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B130" t="n">
+        <v>4006</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>30.03.2023</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F130" t="n">
+        <v>8.359999999999999</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B131" t="n">
+        <v>4007</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>31.03.2023</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F131" t="n">
+        <v>9.02</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B132" t="n">
+        <v>4008</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>31.03.2023</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F132" t="n">
+        <v>11.02</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B133" t="n">
+        <v>107860</v>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>03.04.2023</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F133" t="n">
+        <v>13.46</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B134" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>04.04.2023</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F134" t="n">
+        <v>10.78</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>FC10</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>07.03.2023</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>50000571</v>
+      </c>
+      <c r="F135" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B136" t="n">
+        <v>107896</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F136" t="n">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B137" t="n">
+        <v>29984</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F137" t="n">
+        <v>7.62</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B138" t="n">
+        <v>107908</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F138" t="n">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B139" t="n">
+        <v>15618</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>10008828</v>
+      </c>
+      <c r="F139" t="n">
+        <v>28.32</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B140" t="n">
+        <v>192116</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>10012717</v>
+      </c>
+      <c r="F140" t="n">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B141" t="n">
+        <v>192110</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F141" t="n">
+        <v>8.06</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B142" t="n">
+        <v>192085</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>01.04.2023</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>10012713</v>
+      </c>
+      <c r="F142" t="n">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B143" t="n">
+        <v>4013</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F143" t="n">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B144" t="n">
+        <v>4018</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F144" t="n">
+        <v>9.92</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B145" t="n">
+        <v>4016</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F145" t="n">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B146" t="n">
+        <v>107931</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F146" t="n">
+        <v>10.84</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B147" t="n">
+        <v>192125</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>10010134</v>
+      </c>
+      <c r="F147" t="n">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B148" t="n">
+        <v>219</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>10007154</v>
+      </c>
+      <c r="F148" t="n">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B149" t="n">
+        <v>220</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>10012032</v>
+      </c>
+      <c r="F149" t="n">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B150" t="n">
+        <v>96584</v>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>13.04.2023</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F150" t="n">
+        <v>5.12</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B151" t="n">
+        <v>96525</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>11.04.2023</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F151" t="n">
+        <v>7.66</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B152" t="n">
+        <v>107972</v>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>13.04.2023</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F152" t="n">
+        <v>10.84</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B153" t="n">
+        <v>190947</v>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>22.02.2023</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>10010134</v>
+      </c>
+      <c r="F153" t="n">
+        <v>-8.56</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B154" t="n">
+        <v>192472</v>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>16.04.2023</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>10004464</v>
+      </c>
+      <c r="F154" t="n">
+        <v>6.86</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B155" t="n">
+        <v>192475</v>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>17.04.2023</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>10004822</v>
+      </c>
+      <c r="F155" t="n">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B156" t="n">
+        <v>4026</v>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>14.04.2023</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F156" t="n">
+        <v>11.26</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B157" t="n">
+        <v>4030</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>17.04.2023</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F157" t="n">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B158" t="n">
+        <v>228</v>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>10007154</v>
+      </c>
+      <c r="F158" t="n">
+        <v>5.06</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B159" t="n">
+        <v>11464</v>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>19.04.2023</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>10012279</v>
+      </c>
+      <c r="F159" t="n">
+        <v>6.28</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B160" t="n">
+        <v>11449</v>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>10012279</v>
+      </c>
+      <c r="F160" t="n">
+        <v>4.14</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B161" t="n">
+        <v>10819</v>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>19.04.2023</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F161" t="n">
+        <v>9.699999999999999</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B162" t="n">
+        <v>4028</v>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>14.04.2023</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F162" t="n">
+        <v>9.140000000000001</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B163" t="n">
+        <v>4027</v>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>14.04.2023</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F163" t="n">
+        <v>14.12</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B164" t="n">
+        <v>4021</v>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>12.04.2023</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F164" t="n">
+        <v>11.58</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B165" t="n">
+        <v>223</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>12.04.2023</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>10011068</v>
+      </c>
+      <c r="F165" t="n">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B166" t="n">
+        <v>222</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>12.04.2023</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>10012032</v>
+      </c>
+      <c r="F166" t="n">
+        <v>6.92</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B167" t="n">
+        <v>15690</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>17.04.2023</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>10008828</v>
+      </c>
+      <c r="F167" t="n">
+        <v>29.02</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B168" t="n">
+        <v>10024</v>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>14.04.2023</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>10008243</v>
+      </c>
+      <c r="F168" t="n">
+        <v>22.64</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B169" t="n">
+        <v>225</v>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>13.04.2023</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>10012279</v>
+      </c>
+      <c r="F169" t="n">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B170" t="n">
+        <v>192454</v>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>12.04.2023</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>10012201</v>
+      </c>
+      <c r="F170" t="n">
+        <v>9.52</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B171" t="n">
+        <v>192118</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>10012183</v>
+      </c>
+      <c r="F171" t="n">
+        <v>11.74</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B172" t="n">
+        <v>191719</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>21.03.2023</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>10012745</v>
+      </c>
+      <c r="F172" t="n">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B173" t="n">
+        <v>191720</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>21.03.2023</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>10004759</v>
+      </c>
+      <c r="F173" t="n">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>FC7309</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>10004777</v>
+      </c>
+      <c r="F174" t="n">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B175" t="n">
+        <v>191320</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>02.03.2023</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>10004777</v>
+      </c>
+      <c r="F175" t="n">
+        <v>-6.68</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B176" t="n">
+        <v>191683</v>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>13.03.2023</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>10004777</v>
+      </c>
+      <c r="F176" t="n">
+        <v>-6.58</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B177" t="n">
+        <v>191706</v>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>17.03.2023</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>10004777</v>
+      </c>
+      <c r="F177" t="n">
+        <v>-6.58</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B178" t="n">
+        <v>192062</v>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>28.03.2023</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>10004777</v>
+      </c>
+      <c r="F178" t="n">
+        <v>-6.46</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B179" t="n">
+        <v>24432</v>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>10007342</v>
+      </c>
+      <c r="F179" t="n">
+        <v>10.52</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B180" t="n">
+        <v>15691</v>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>10008828</v>
+      </c>
+      <c r="F180" t="n">
+        <v>28.08</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B181" t="n">
+        <v>108030</v>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F181" t="n">
+        <v>8.76</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B182" t="n">
+        <v>11480</v>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>10012279</v>
+      </c>
+      <c r="F182" t="n">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B183" t="n">
+        <v>4034</v>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>19.04.2023</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F183" t="n">
+        <v>11.08</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B184" t="n">
+        <v>4036</v>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F184" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B185" t="n">
+        <v>4036</v>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F185" t="n">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B186" t="n">
+        <v>4035</v>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F186" t="n">
+        <v>7.58</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B187" t="n">
+        <v>4037</v>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F187" t="n">
+        <v>9.98</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B188" t="n">
+        <v>15691</v>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>10008828</v>
+      </c>
+      <c r="F188" t="n">
+        <v>28.08</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B189" t="n">
+        <v>8</v>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>50000571</v>
+      </c>
+      <c r="F189" t="n">
+        <v>10.52</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B190" t="n">
+        <v>9</v>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>50000571</v>
+      </c>
+      <c r="F190" t="n">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B191" t="n">
+        <v>192503</v>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>10004822</v>
+      </c>
+      <c r="F191" t="n">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B192" t="n">
+        <v>4039</v>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>25.04.2023</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F192" t="n">
+        <v>10.04</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B193" t="n">
+        <v>15755</v>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>25.04.2023</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>10008828</v>
+      </c>
+      <c r="F193" t="n">
+        <v>28.26</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B194" t="n">
+        <v>108078</v>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>25.04.2023</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>80000043</v>
+      </c>
+      <c r="F194" t="n">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B195" t="n">
+        <v>4043</v>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F195" t="n">
+        <v>10.58</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B196" t="n">
+        <v>192500</v>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>10005092</v>
+      </c>
+      <c r="F196" t="n">
+        <v>8.800000000000001</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B197" t="n">
+        <v>192518</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>25.04.2023</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>10012717</v>
+      </c>
+      <c r="F197" t="n">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B198" t="n">
+        <v>192497</v>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>10012183</v>
+      </c>
+      <c r="F198" t="n">
+        <v>9.359999999999999</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B199" t="n">
+        <v>192850</v>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>10012257</v>
+      </c>
+      <c r="F199" t="n">
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B200" t="n">
+        <v>4050</v>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>28.04.2023</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F200" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B201" t="n">
+        <v>4047</v>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F201" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>10002770</v>
+      </c>
+      <c r="B202" t="n">
+        <v>12897</v>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>10004686</v>
+      </c>
+      <c r="F202" t="n">
+        <v>18.94</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B205" t="n">
+        <v>8185</v>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>01.03.2023</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F205" t="n">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B206" t="n">
+        <v>8186</v>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>01.03.2023</t>
+        </is>
+      </c>
+      <c r="E206" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F206" t="n">
+        <v>17.68</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B207" t="n">
+        <v>8188</v>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>02.03.2023</t>
+        </is>
+      </c>
+      <c r="E207" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F207" t="n">
+        <v>17.32</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B208" t="n">
+        <v>8194</v>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>06.03.2023</t>
+        </is>
+      </c>
+      <c r="E208" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F208" t="n">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B209" t="n">
+        <v>8203</v>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>09.03.2023</t>
+        </is>
+      </c>
+      <c r="E209" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F209" t="n">
+        <v>17.72</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B210" t="n">
+        <v>8205</v>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>10.03.2023</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F210" t="n">
+        <v>17.46</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B211" t="n">
+        <v>8206</v>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>10.03.2023</t>
+        </is>
+      </c>
+      <c r="E211" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F211" t="n">
+        <v>17.68</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B212" t="n">
+        <v>8209</v>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>13.03.2023</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F212" t="n">
+        <v>16.18</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B213" t="n">
+        <v>8210</v>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>13.03.2023</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F213" t="n">
+        <v>19.44</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B214" t="n">
+        <v>8211</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>14.03.2023</t>
+        </is>
+      </c>
+      <c r="E214" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F214" t="n">
+        <v>18.66</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B215" t="n">
+        <v>8212</v>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>14.03.2023</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F215" t="n">
+        <v>18.42</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B216" t="n">
+        <v>8213</v>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>16.03.2023</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F216" t="n">
+        <v>18.6</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B217" t="n">
+        <v>8214</v>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>16.03.2023</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F217" t="n">
+        <v>18.66</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B218" t="n">
+        <v>8215</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>16.03.2023</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F218" t="n">
+        <v>18.42</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B219" t="n">
+        <v>8224</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>21.03.2023</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F219" t="n">
+        <v>18.52</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B220" t="n">
+        <v>8174</v>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>23.02.2023</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F220" t="n">
+        <v>18.52</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B221" t="n">
+        <v>8180</v>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>27.02.2023</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F221" t="n">
+        <v>17.98</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B222" t="n">
+        <v>8179</v>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>27.02.2023</t>
+        </is>
+      </c>
+      <c r="E222" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F222" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B223" t="n">
+        <v>8184</v>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>28.02.2023</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F223" t="n">
+        <v>18.06</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B224" t="n">
+        <v>8307</v>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>10.04.2023</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F224" t="n">
+        <v>17.22</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B225" t="n">
+        <v>8226</v>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>22.03.2023</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F225" t="n">
+        <v>18.48</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B226" t="n">
+        <v>8232</v>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>23.03.2023</t>
+        </is>
+      </c>
+      <c r="E226" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F226" t="n">
+        <v>18.94</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B227" t="n">
+        <v>8189</v>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>02.03.2023</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F227" t="n">
+        <v>18.18</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B228" t="n">
+        <v>8245</v>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>04.04.2023</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F228" t="n">
+        <v>17.92</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B229" t="n">
+        <v>8243</v>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>03.04.2023</t>
+        </is>
+      </c>
+      <c r="E229" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F229" t="n">
+        <v>18.1</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B230" t="n">
+        <v>8336</v>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="E230" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F230" t="n">
+        <v>18.74</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>10002771</v>
+      </c>
+      <c r="B231" t="n">
+        <v>8339</v>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E231" t="n">
+        <v>10004861</v>
+      </c>
+      <c r="F231" t="n">
+        <v>18.38</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>10002774</v>
+      </c>
+      <c r="B234" t="n">
+        <v>4032</v>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="E234" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F234" t="n">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>10002774</v>
+      </c>
+      <c r="B235" t="n">
+        <v>4017</v>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E235" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F235" t="n">
+        <v>8.24</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>10002774</v>
+      </c>
+      <c r="B236" t="n">
+        <v>4012</v>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>05.04.2023</t>
+        </is>
+      </c>
+      <c r="E236" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F236" t="n">
+        <v>12.72</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>10002774</v>
+      </c>
+      <c r="B237" t="n">
+        <v>4019</v>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>06.04.2023</t>
+        </is>
+      </c>
+      <c r="E237" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F237" t="n">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>10002774</v>
+      </c>
+      <c r="B238" t="n">
+        <v>4023</v>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>13.04.2023</t>
+        </is>
+      </c>
+      <c r="E238" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F238" t="n">
+        <v>12.12</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>10002774</v>
+      </c>
+      <c r="B239" t="n">
+        <v>4036</v>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>21.04.2023</t>
+        </is>
+      </c>
+      <c r="E239" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F239" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>10002774</v>
+      </c>
+      <c r="B240" t="n">
+        <v>4046</v>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="E240" t="n">
+        <v>10004786</v>
+      </c>
+      <c r="F240" t="n">
+        <v>11.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>